<commit_message>
filter some of benchmarks
</commit_message>
<xml_diff>
--- a/benchmark/ncaa-containing_complex.xlsx
+++ b/benchmark/ncaa-containing_complex.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E266F5A4-7891-4C00-A45D-8A55CDB211D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31F5C6-5D13-496B-AF39-D055BA652DF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10.1021/cb400209w</t>
-  </si>
-  <si>
     <t>Selective detection of caspase-3 versus caspase-7 using activity-based probes with key unnatural amino acids</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t>caspase-3</t>
-  </si>
-  <si>
-    <t>10.1021/cb5004256</t>
   </si>
   <si>
     <t>caspase-8/9</t>
@@ -757,63 +751,72 @@
     <t>Discovery of potent antagonists of the antiapoptotic protein XIAP for the treatment of cancer</t>
   </si>
   <si>
+    <t>1TFT</t>
+  </si>
+  <si>
+    <t>screening experiment based on a peptide motif AVP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">with a tetrahydronaphthyl amide cap at C terminal </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha-tert-butyl-Gly,4-phenoxy-proline,etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discovery of a Potent Small-Molecule Antagonist of Inhibitor of Apoptosis (IAP) Proteins and Clinical Candidate for the Treatment of Cancer (GDC-0152)</t>
+  </si>
+  <si>
+    <t>10.1021/jm300060k</t>
+  </si>
+  <si>
+    <t>3UW5</t>
+  </si>
+  <si>
+    <t>alpha-cyclohexyl-Gly,trans-3-methyl-proline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha-cyclohexyl-Gly,etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with a thiadiazole at N terminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4- difluorocyclohexyl,etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4HY0</t>
+  </si>
+  <si>
+    <t>10.1021/jm301674z</t>
+  </si>
+  <si>
+    <t>Design and Synthesis of Potent Inhibitor of Apoptosis (IAP) Proteins Antagonists Bearing an Octahydropyrrolo[1,2-a]pyrazine Scaffold as a Novel Proline Mimetic</t>
+  </si>
+  <si>
+    <t>screening experiment based on a peptide motif AVPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with a dihydronaphthalen group at C terminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1021/cb400209w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1021/cb5004256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>10.1021/jm040037k</t>
-  </si>
-  <si>
-    <t>1TFT</t>
-  </si>
-  <si>
-    <t>screening experiment based on a peptide motif AVP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">with a tetrahydronaphthyl amide cap at C terminal </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alpha-tert-butyl-Gly,4-phenoxy-proline,etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Discovery of a Potent Small-Molecule Antagonist of Inhibitor of Apoptosis (IAP) Proteins and Clinical Candidate for the Treatment of Cancer (GDC-0152)</t>
-  </si>
-  <si>
-    <t>10.1021/jm300060k</t>
-  </si>
-  <si>
-    <t>3UW5</t>
-  </si>
-  <si>
-    <t>alpha-cyclohexyl-Gly,trans-3-methyl-proline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>alpha-cyclohexyl-Gly,etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>with a thiadiazole at N terminal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4,4- difluorocyclohexyl,etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4HY0</t>
-  </si>
-  <si>
-    <t>10.1021/jm301674z</t>
-  </si>
-  <si>
-    <t>Design and Synthesis of Potent Inhibitor of Apoptosis (IAP) Proteins Antagonists Bearing an Octahydropyrrolo[1,2-a]pyrazine Scaffold as a Novel Proline Mimetic</t>
-  </si>
-  <si>
-    <t>screening experiment based on a peptide motif AVPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>with a dihydronaphthalen group at C terminal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1168,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1206,13 +1209,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -1223,31 +1226,31 @@
         <v>2013</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1255,31 +1258,31 @@
         <v>2014</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1287,31 +1290,31 @@
         <v>2014</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G4" s="1">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
@@ -1319,28 +1322,28 @@
         <v>2017</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1348,28 +1351,28 @@
         <v>2018</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
@@ -1377,31 +1380,31 @@
         <v>2012</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1409,31 +1412,31 @@
         <v>2015</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G8" s="1">
         <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1441,28 +1444,28 @@
         <v>2018</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1470,31 +1473,31 @@
         <v>2021</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1502,31 +1505,31 @@
         <v>2016</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" s="1">
-        <v>4</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="L11" s="1"/>
     </row>
@@ -1535,28 +1538,28 @@
         <v>2012</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="G12" s="1">
         <v>5</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L12" s="1"/>
     </row>
@@ -1565,28 +1568,28 @@
         <v>2012</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L13" s="1"/>
     </row>
@@ -1595,31 +1598,31 @@
         <v>2009</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G14" s="1">
         <v>4</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1627,31 +1630,31 @@
         <v>2004</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G15" s="1">
         <v>4</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1659,31 +1662,31 @@
         <v>2012</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G16" s="1">
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1691,31 +1694,31 @@
         <v>2012</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G17" s="1">
         <v>3</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1723,25 +1726,25 @@
         <v>2016</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L19" s="1"/>
     </row>
@@ -1750,25 +1753,25 @@
         <v>2011</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L20" s="1"/>
     </row>
@@ -1777,31 +1780,31 @@
         <v>2013</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="K21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L21" s="1"/>
     </row>
@@ -1810,28 +1813,28 @@
         <v>2011</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L22" s="1"/>
     </row>
@@ -1840,31 +1843,31 @@
         <v>2016</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L23" s="1"/>
     </row>
@@ -1873,31 +1876,31 @@
         <v>2019</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L24" s="1"/>
     </row>

</xml_diff>

<commit_message>
finish filtering of all benchmarks
</commit_message>
<xml_diff>
--- a/benchmark/ncaa-containing_complex.xlsx
+++ b/benchmark/ncaa-containing_complex.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31F5C6-5D13-496B-AF39-D055BA652DF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5C67DF-2EA5-4A7C-B010-801608FAF3B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,14 +632,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FITC group at C terminal for fluorescently labeled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FITC group for fluorescently labeled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Rational Design and Characterization of D-Phe-Pro-D-Arg-Derived Direct Thrombin Inhibitors</t>
   </si>
   <si>
@@ -794,29 +786,38 @@
     <t>4HY0</t>
   </si>
   <si>
+    <t>Design and Synthesis of Potent Inhibitor of Apoptosis (IAP) Proteins Antagonists Bearing an Octahydropyrrolo[1,2-a]pyrazine Scaffold as a Novel Proline Mimetic</t>
+  </si>
+  <si>
+    <t>screening experiment based on a peptide motif AVPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with a dihydronaphthalen group at C terminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1021/cb400209w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1021/cb5004256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1021/jm040037k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constrained peptide; FITC group for fluorescently labeled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stapled peptide; FITC group at C terminal for fluorescently labeled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>10.1021/jm301674z</t>
-  </si>
-  <si>
-    <t>Design and Synthesis of Potent Inhibitor of Apoptosis (IAP) Proteins Antagonists Bearing an Octahydropyrrolo[1,2-a]pyrazine Scaffold as a Novel Proline Mimetic</t>
-  </si>
-  <si>
-    <t>screening experiment based on a peptide motif AVPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>with a dihydronaphthalen group at C terminal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.1021/cb400209w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.1021/cb5004256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.1021/jm040037k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -824,7 +825,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,13 +866,39 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -883,15 +910,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="适中" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1172,7 +1209,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,9 +1263,9 @@
         <v>2013</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1258,9 +1295,9 @@
         <v>2014</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1305,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="G4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>66</v>
@@ -1314,7 +1351,7 @@
         <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.35">
@@ -1337,7 +1374,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>66</v>
@@ -1353,7 +1390,7 @@
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1382,7 +1419,7 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1414,7 +1451,7 @@
       <c r="B8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1427,7 +1464,7 @@
         <v>76</v>
       </c>
       <c r="G8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>30</v>
@@ -1529,7 +1566,7 @@
         <v>107</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="L11" s="1"/>
     </row>
@@ -1538,19 +1575,19 @@
         <v>2012</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="G12" s="1">
         <v>5</v>
@@ -1559,7 +1596,7 @@
         <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L12" s="1"/>
     </row>
@@ -1568,28 +1605,28 @@
         <v>2012</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L13" s="1"/>
     </row>
@@ -1598,19 +1635,19 @@
         <v>2009</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G14" s="1">
         <v>4</v>
@@ -1619,10 +1656,10 @@
         <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1630,19 +1667,19 @@
         <v>2004</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>133</v>
+        <v>149</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G15" s="1">
         <v>4</v>
@@ -1651,10 +1688,10 @@
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1662,19 +1699,19 @@
         <v>2012</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G16" s="1">
         <v>4</v>
@@ -1683,10 +1720,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1694,31 +1731,31 @@
         <v>2012</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1726,16 +1763,16 @@
         <v>2016</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -1744,7 +1781,7 @@
         <v>48</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L19" s="1"/>
     </row>
@@ -1795,7 +1832,7 @@
         <v>49</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>48</v>
@@ -1858,7 +1895,7 @@
         <v>60</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>48</v>
@@ -1891,7 +1928,7 @@
         <v>71</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>48</v>

</xml_diff>